<commit_message>
@all: Worked on the submit functionality
</commit_message>
<xml_diff>
--- a/src/SubscriptionExpirySample.xlsx
+++ b/src/SubscriptionExpirySample.xlsx
@@ -20,12 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">ICCID</t>
   </si>
   <si>
-    <t xml:space="preserve">Sim2ExpiryDate</t>
+    <t xml:space="preserve">Expiry Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">###</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DD/MM/YYYY</t>
   </si>
   <si>
     <t xml:space="preserve">8991102105546012952F</t>
@@ -38,7 +44,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -76,6 +82,7 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -120,7 +127,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -155,10 +162,6 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -241,7 +244,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -262,17 +265,21 @@
       <c r="C1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="n">
-        <v>45471</v>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
       </c>
       <c r="C2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9"/>
-      <c r="B3" s="6"/>
+      <c r="A3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="8" t="n">
+        <v>45471</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
@all : Added another condition for partial successful updates in the simManagement.js file | Changed the position of the responseMessage, Added a state to keep track of date validation messages on file change, Added another condition for date object on file change in the ImportExcel.js file
</commit_message>
<xml_diff>
--- a/src/SubscriptionExpirySample.xlsx
+++ b/src/SubscriptionExpirySample.xlsx
@@ -20,21 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">ICCID</t>
   </si>
   <si>
-    <t xml:space="preserve">Expiry Date</t>
+    <t xml:space="preserve">Expiry Date (DD/MM/YYYY)</t>
   </si>
   <si>
-    <t xml:space="preserve">###</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DD/MM/YYYY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8991102105546012952F</t>
+    <t xml:space="preserve">8991102105546012952F </t>
   </si>
 </sst>
 </file>
@@ -46,7 +40,7 @@
     <numFmt numFmtId="165" formatCode="#,##0"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -75,13 +69,6 @@
       <color rgb="FF61576E"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -127,7 +114,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -156,11 +143,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -241,10 +224,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -264,23 +247,16 @@
       </c>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="6"/>
+      <c r="B2" s="7" t="n">
+        <v>46690</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="8" t="n">
-        <v>45471</v>
-      </c>
-    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
@All : Changed the date format to text in excel sheet, Added new function to check the format of date string, Changed the onFileChange function's conditions for checking & setting the expiry date, And Updated the rendering of the expiry date from frontend & backend
</commit_message>
<xml_diff>
--- a/src/SubscriptionExpirySample.xlsx
+++ b/src/SubscriptionExpirySample.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -10,17 +10,17 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">ICCID</t>
   </si>
@@ -28,25 +28,25 @@
     <t xml:space="preserve">Expiry Date (DD/MM/YYYY)</t>
   </si>
   <si>
-    <t xml:space="preserve">8991102105546012952F </t>
+    <t xml:space="preserve">8991102105546012952F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24/10/2026</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -65,10 +65,10 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF61576E"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="12"/>
+      <color rgb="BF333333"/>
+      <name val="ariel"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -114,37 +114,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -204,7 +188,7 @@
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF61576E"/>
+      <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
@@ -213,7 +197,7 @@
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="BF333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -224,46 +208,41 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1048576"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="21.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1018" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.35"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="n">
-        <v>46690</v>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>